<commit_message>
Still need to finish SOCOCV at N30
</commit_message>
<xml_diff>
--- a/data/Lab2_data/HPPC_import/N30.xlsx
+++ b/data/Lab2_data/HPPC_import/N30.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Desktop\Lab_2\Modle\Project_Lab2\Lab_2\data\Lab2_data\HPPC_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016584B3-297E-4441-A0CF-DA1D298D002B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46C1181-69CC-4627-B84D-64FD9F1B5F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18654,8 +18654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B7F80E-682C-4B5D-B163-4CA3970493A9}">
   <dimension ref="A1:D819"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A802" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O822" sqref="O822"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30243,7 +30243,7 @@
         <v>17797</v>
       </c>
       <c r="B773">
-        <f t="shared" ref="B773:B836" si="12">A773-32</f>
+        <f t="shared" ref="B773:B819" si="12">A773-32</f>
         <v>17765</v>
       </c>
       <c r="C773">

</xml_diff>